<commit_message>
[#1199980645336559] fixed input for test case g
</commit_message>
<xml_diff>
--- a/pentaho/test/SP-0.2/test-case-G/inputs/input.xlsx
+++ b/pentaho/test/SP-0.2/test-case-G/inputs/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon.ecung\Projects\data-warehouse\pentaho\test\SP-0.1\test-case-G\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon.ecung\Projects\data-warehouse\pentaho\test\SP-0.2\test-case-G\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34ABED94-A2F1-4A45-8AA0-3D14BBE50D19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5A95E-7470-4334-A2FE-BD1282CEBBE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="7515" windowWidth="13800" windowHeight="9360"/>
+    <workbookView xWindow="5955" yWindow="7515" windowWidth="13800" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>tool_pid</t>
   </si>
@@ -45,11 +45,17 @@
   <si>
     <t>Ladder</t>
   </si>
+  <si>
+    <t>extra_column</t>
+  </si>
+  <si>
+    <t>extra_column_data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -884,14 +890,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,8 +918,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -926,6 +937,9 @@
       </c>
       <c r="E2" s="1">
         <v>30825</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>